<commit_message>
#744 #745 #748 #749 #750 #751 #754 #762 테스트케이스_작성양식.xlsx TC0001~TC0015까지 작성
</commit_message>
<xml_diff>
--- a/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스_작성양식.xlsx
+++ b/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스_작성양식.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aqua9\Desktop\테스트케이스 및 테스트결과보고서\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="이력" sheetId="2" r:id="rId1"/>
     <sheet name="테스트케이스" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="127">
   <si>
     <t>TestCase ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,10 +74,6 @@
   </si>
   <si>
     <t>Test Case</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt; 팀 명&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -159,12 +150,476 @@
 예) TC-0001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>UC001
+UC008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목 등록 버튼의 작동 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목 등록 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목명
+담당교수
+강의 요일, 강의 시작시간,종료시간
+수강년도, 수강학기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 과목명을 입력한다.
+2. 담당교수를 입력한다.
+3. 강의 요일, 강의 시작 시간, 종료 시간을 입력한다.
+4. 수강년도, 수강학기를 입력한다.
+5. 과목 등록 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입력한 값들이 모두 에러없이
+메인화면의 시간표에 출력된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC001
+UC019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목명 미입력 시 에러 메시지 출력 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목명을 제외한 나머지 값들은 정확히 입력
+하고 과목 등록 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>담당교수, 강의 요일, 강의 시작시간, 
+강의 종료시간, 수강년도, 수강학기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 과목명을 입력하지않는다.
+2. 과목명을 제외한 나머지 값들을 정확히 입력한다.
+3. 과목 등록 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목명 공백에 대한 에러 메시지가 출력된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목 등록 시 중복된 정보 입력에 대한
+에러 메시지 출력 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미 등록된 과목명 또는 강의 시간을 입력하고 과목 등록 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 과목명 또는 강의 시간을  이미 등록된 정보로 입력한다.
+2. 나머지 값들은 정확히 입력한다.
+3. 과목 등록 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중복된 정보 입력에 대한 에러
+메시지가 출력된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC002
+UC008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목 수정 버튼의 작동 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">과목 수정 버튼을 클릭한다.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 메인화면의 시간표에서 수정할 과목을 선택하여 과목관리 버튼을 누른다.
+2. 수정할 내용을 입력한다.
+3. 수정 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입력한 값들이 에러없이 수정되어 메인화면에 출력된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC002
+UC008
+UC019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목 수정 시 이미 등록된 과목과 중복된 
+정보 입력에 대한 에러 메시지 출력 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미 등록된 과목명 또는 강의 시간을 입력 하고 과목 수정 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 메인화면의 시간표에서 수정할 과목을 선택하여 과목관리 버튼을 클릭한다.
+2. 과목명 또는 강의 시간을 이미 등록된 정보로 입력한다.
+3. 수정 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인화면 시간표에서 빈 공간 선택 후 과목 
+수정 버튼 클릭 시 에러 메시지 출력 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 메인화면의 시간표에서 빈
+공간을 선택하여 과목 관리 
+버튼을 클릭한다.
+2. 모든 입력값을 정확히 입력
+한다.
+3. 수정 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록되지 않은 과목 수정 불가에 대한 에러 메세지가 출력된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC008
+UC011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목별 todo 관리 화면 띄우기 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 화면 시간표의 과목을 더블 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>더블 클릭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. To do 관리를 원하는 
+과목을 더블 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목별 To do 관리 화면이 
+실행된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC008
+UC011
+UC019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 화면 시간표에서 빈 공간 더블 클릭 시
+에러 메시지 출력 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 화면 시간표의 빈 공간을 더블 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 과목이 등록되어있지 않은
+빈 공간을 더블 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목별 To do 관리 화면은 출력되지않고, 빈 공간 선택에 대한 에러 메세지가 출력된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC005
+UC011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>todo 등록 버튼 에러 없이 작동 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>todo 등록 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>항목명
+마감기한(년,월,일,시,분)
+실제마감일(년,월,일,시,분)
+완료 여부, 중요 여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 항목명을 입력한다.
+2. 마감기한(년,월,일,시,분)을 입력한다.
+3. 실제마감일(년,월,일,시,분)을 입력한다.
+4. 완료 여부와 중요 여부를 체크한다.
+5. To do 등록 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입력한 값들이 모두 에러없이 
+과목별 To do 관리 화면에 출력된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC005
+UC011
+UC019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>항목명 미입력 시 에러 메시지 출력 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>항목명을 제외한 나머지 값들은 정확히 
+입력하고 To do 등록 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마감기한(년,월,일,시,분)
+실제마감일(년,월,일,시,분)
+완료 여부,중요 여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 항목명을 입력하지 않는다.
+2. 마감기한, 실제마감일, 완료 여부, 중요 여부를 정확히 입력한다.
+3. To do 등록 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>항목명 미입력에 대한 에러 메시지가 출력된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘못된 마감기한 입력 시 에러 메시지 출력 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마감기한을 제외한 나머지 값들은 정확히
+입력하고 To do 등록 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>항목명
+잘못된 마감기한
+실제마감일
+완료 여부, 중요 여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 마감기한을 제외한 모든 정보를 정확히 입력한다.
+2. 잘못된 마감기한을 입력한다.
+3. To do 등록 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>날짜 오류에 대한 에러 메시지가 출력된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC006
+UC011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목별 todo 수정 버튼 에러 없이 작동 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">todo 수정 버튼을 클릭한다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>항목명
+마감기한(년,월,일,시,분)
+실제마감일(년,월,일,시,분)
+완료 여부, 중요 여부 중 
+수정을 원하는 내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 수정할 To do를 선택한다.
+2. 수정할 내용을 입력 후 To do 수정 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입력한 값들이 모두 에러없이 수정되어 과목별 To do 관리 화면에 출력된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC007
+UC011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>todo 삭제 버튼 에러 없이 작동 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>todo 삭제 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삭제할 To do를 클릭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 삭제할 To do를 선택한다.
+2. To do 삭제 버튼을 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">선택한 To do가 과목별 To do 관리 화면에서 삭제된다.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UC011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목별 todo 완료여부 체크박스 작동확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목별 todo 화면을 띄운다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완료 여부 체크박스 클릭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 완료한 To do의 완료 여부
+체크박스를 클릭한다.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실제 마감일이 에러없이 
+과목별 To do 관리 화면에 출력된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과목별 todo 중요여부 체크박스 작동확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중요 여부 체크박스 클릭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 중요한 To do의 중요 여부 
+체크박스를 클릭한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중요 여부가 체크된 To do의 
+색이 노란색으로 출력된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.06.05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정화인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt; 4조 Tuna&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0001~TC-0015 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,7 +717,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -444,13 +899,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -525,6 +991,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -586,7 +1064,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -638,7 +1116,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -832,178 +1310,188 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="4" width="15.625" customWidth="1"/>
+    <col min="1" max="2" width="15.58203125" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="41.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="39.5">
       <c r="B1" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="7.5" customHeight="1"/>
+    <row r="3" spans="1:4" ht="6.75" customHeight="1"/>
+    <row r="4" spans="1:4" ht="21">
+      <c r="D4" s="23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="54" customHeight="1"/>
+    <row r="6" spans="1:4" ht="23.25" customHeight="1">
+      <c r="A6" s="24" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="D4" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
-        <v>28</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
     </row>
-    <row r="7" spans="1:4" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="4.5" customHeight="1" thickBot="1">
       <c r="B7" s="21"/>
     </row>
-    <row r="8" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="17.5" thickBot="1">
       <c r="A8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="C8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="D8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="15">
+        <v>1</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="9"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="9"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="9"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="9"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="9"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="9"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="9"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="9"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="9"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="9"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="9"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21" s="9"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="9"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" s="9"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" s="9"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4">
       <c r="A25" s="9"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4">
       <c r="A26" s="9"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4">
       <c r="A27" s="9"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="17.5" thickBot="1">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -1020,55 +1508,55 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="5.25" customWidth="1"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="16.58203125" customWidth="1"/>
     <col min="3" max="3" width="17.75" customWidth="1"/>
     <col min="4" max="4" width="35.5" customWidth="1"/>
-    <col min="5" max="5" width="30.75" customWidth="1"/>
-    <col min="6" max="6" width="17.75" customWidth="1"/>
-    <col min="7" max="7" width="25.75" customWidth="1"/>
-    <col min="8" max="8" width="26.625" customWidth="1"/>
+    <col min="5" max="5" width="38.1640625" customWidth="1"/>
+    <col min="6" max="6" width="24.9140625" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" customWidth="1"/>
+    <col min="8" max="8" width="26.58203125" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="11.875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" style="7" customWidth="1"/>
     <col min="11" max="11" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="30">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="21.75" customHeight="1">
       <c r="B7" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>0</v>
@@ -1077,7 +1565,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>2</v>
@@ -1098,219 +1586,429 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="85">
       <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="D8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="G8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+    <row r="9" spans="1:11" ht="119">
+      <c r="B9" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>36</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="8"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+    <row r="10" spans="1:11" ht="68">
+      <c r="B10" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>43</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="8"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+    <row r="11" spans="1:11" ht="85">
+      <c r="B11" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>48</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="8"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+    <row r="12" spans="1:11" ht="85">
+      <c r="B12" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="8"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+    <row r="13" spans="1:11" ht="102">
+      <c r="B13" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>48</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="8"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+    <row r="14" spans="1:11" ht="102">
+      <c r="B14" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>63</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="8"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+    <row r="15" spans="1:11" ht="34">
+      <c r="B15" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>70</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="8"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+    <row r="16" spans="1:11" ht="51">
+      <c r="B16" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>76</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="8"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+    <row r="17" spans="2:11" ht="153">
+      <c r="B17" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>83</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="8"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+    <row r="18" spans="2:11" ht="102">
+      <c r="B18" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>90</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="8"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+    <row r="19" spans="2:11" ht="102">
+      <c r="B19" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>96</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="8"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+    <row r="20" spans="2:11" ht="136">
+      <c r="B20" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>103</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="8"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+    <row r="21" spans="2:11" ht="51">
+      <c r="B21" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>110</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="8"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+    <row r="22" spans="2:11" ht="51">
+      <c r="B22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>117</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="8"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+    <row r="23" spans="2:11" ht="34">
+      <c r="B23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>122</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="8"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1322,7 +2020,7 @@
       <c r="J24" s="8"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1334,7 +2032,7 @@
       <c r="J25" s="8"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1346,7 +2044,7 @@
       <c r="J26" s="8"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>

</xml_diff>

<commit_message>
#744 #745 #748 #749 #750 #751 #754 #762 테스트케이스_작성양식.xlsx TC0001~TC0015 테스트
</commit_message>
<xml_diff>
--- a/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스_작성양식.xlsx
+++ b/doc/4_ 테스트케이스 및 테스트결과보고서/테스트케이스_작성양식.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eunho\SE2017_4_tuna\doc\4_ 테스트케이스 및 테스트결과보고서\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="이력" sheetId="2" r:id="rId1"/>
     <sheet name="테스트케이스" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="243">
   <si>
     <t>TestCase ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1085,12 +1080,55 @@
     <t>김은호</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fail
+빈 공간 선택에 대한 에러 메시지가 출력되지 않음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fail
+항목명 미입력에 대한 에러 메시지가 출력되지않음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fail 
+등록되지 않은 과목 수정 불가에 대한 에러 메시지가 출력되지않음.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#939</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#940</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#941</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017.06.05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC-0001~TC-0015 테스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정화인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1806,41 +1844,41 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="2" width="15.625" customWidth="1"/>
-    <col min="3" max="3" width="21.625" customWidth="1"/>
-    <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="1" max="2" width="15.58203125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="41.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="39.5">
       <c r="B1" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="7.5" customHeight="1"/>
+    <row r="3" spans="1:4" ht="6.75" customHeight="1"/>
+    <row r="4" spans="1:4" ht="21">
       <c r="D4" s="23" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="54" customHeight="1"/>
+    <row r="6" spans="1:4" ht="23.25" customHeight="1">
       <c r="A6" s="31" t="s">
         <v>27</v>
       </c>
@@ -1848,10 +1886,10 @@
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
     </row>
-    <row r="7" spans="1:4" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="4.5" customHeight="1" thickBot="1">
       <c r="B7" s="21"/>
     </row>
-    <row r="8" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="17.5" thickBot="1">
       <c r="A8" s="17" t="s">
         <v>14</v>
       </c>
@@ -1865,7 +1903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="14" t="s">
         <v>123</v>
       </c>
@@ -1879,7 +1917,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="9" t="s">
         <v>230</v>
       </c>
@@ -1893,109 +1931,117 @@
         <v>232</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
+      <c r="A11" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="9"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="9"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="9"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="9"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="9"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="9"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="9"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="9"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="9"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21" s="9"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="9"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" s="9"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" s="9"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4">
       <c r="A25" s="9"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4">
       <c r="A26" s="9"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4">
       <c r="A27" s="9"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="17.5" thickBot="1">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -2012,35 +2058,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="5.25" customWidth="1"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="16.58203125" customWidth="1"/>
     <col min="3" max="3" width="17.75" customWidth="1"/>
     <col min="4" max="4" width="56" customWidth="1"/>
-    <col min="5" max="5" width="38.125" customWidth="1"/>
-    <col min="6" max="6" width="28.125" customWidth="1"/>
+    <col min="5" max="5" width="38.08203125" customWidth="1"/>
+    <col min="6" max="6" width="28.08203125" customWidth="1"/>
     <col min="7" max="7" width="54" customWidth="1"/>
-    <col min="8" max="8" width="49.125" customWidth="1"/>
+    <col min="8" max="8" width="49.08203125" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
-    <col min="10" max="10" width="11.875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" style="7" customWidth="1"/>
     <col min="11" max="11" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="30">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
@@ -2048,13 +2094,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -2062,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="21.75" customHeight="1">
       <c r="B7" s="22" t="s">
         <v>21</v>
       </c>
@@ -2094,7 +2140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="85">
       <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
@@ -2126,7 +2172,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="85">
       <c r="B9" s="24" t="s">
         <v>30</v>
       </c>
@@ -2148,11 +2194,15 @@
       <c r="H9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="8"/>
+      <c r="I9" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J9" s="28">
+        <v>42891</v>
+      </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="66" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="68">
       <c r="B10" s="24" t="s">
         <v>37</v>
       </c>
@@ -2174,11 +2224,15 @@
       <c r="H10" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="8"/>
+      <c r="I10" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J10" s="28">
+        <v>42891</v>
+      </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="85">
       <c r="B11" s="24" t="s">
         <v>37</v>
       </c>
@@ -2200,11 +2254,15 @@
       <c r="H11" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="8"/>
+      <c r="I11" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J11" s="28">
+        <v>42891</v>
+      </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="85">
       <c r="B12" s="24" t="s">
         <v>49</v>
       </c>
@@ -2226,11 +2284,15 @@
       <c r="H12" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="8"/>
+      <c r="I12" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J12" s="28">
+        <v>42891</v>
+      </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="85">
       <c r="B13" s="24" t="s">
         <v>55</v>
       </c>
@@ -2252,11 +2314,15 @@
       <c r="H13" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="8"/>
+      <c r="I13" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J13" s="28">
+        <v>42891</v>
+      </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="99" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="102">
       <c r="B14" s="24" t="s">
         <v>55</v>
       </c>
@@ -2278,11 +2344,17 @@
       <c r="H14" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="I14" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="J14" s="28">
+        <v>42891</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="34">
       <c r="B15" s="24" t="s">
         <v>64</v>
       </c>
@@ -2304,11 +2376,15 @@
       <c r="H15" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="8"/>
+      <c r="I15" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J15" s="28">
+        <v>42891</v>
+      </c>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="68">
       <c r="B16" s="24" t="s">
         <v>71</v>
       </c>
@@ -2330,11 +2406,17 @@
       <c r="H16" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="2:11" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="I16" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="J16" s="28">
+        <v>42891</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="85">
       <c r="B17" s="24" t="s">
         <v>77</v>
       </c>
@@ -2356,11 +2438,15 @@
       <c r="H17" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="8"/>
+      <c r="I17" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J17" s="28">
+        <v>42891</v>
+      </c>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" ht="68">
       <c r="B18" s="24" t="s">
         <v>84</v>
       </c>
@@ -2382,11 +2468,17 @@
       <c r="H18" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="I18" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="J18" s="28">
+        <v>42891</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="68">
       <c r="B19" s="24" t="s">
         <v>84</v>
       </c>
@@ -2408,11 +2500,15 @@
       <c r="H19" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="8"/>
+      <c r="I19" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J19" s="28">
+        <v>42891</v>
+      </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="2:11" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" ht="85">
       <c r="B20" s="24" t="s">
         <v>97</v>
       </c>
@@ -2434,11 +2530,15 @@
       <c r="H20" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="8"/>
+      <c r="I20" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J20" s="28">
+        <v>42891</v>
+      </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" ht="34">
       <c r="B21" s="24" t="s">
         <v>104</v>
       </c>
@@ -2460,11 +2560,15 @@
       <c r="H21" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="8"/>
+      <c r="I21" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J21" s="28">
+        <v>42891</v>
+      </c>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" ht="51">
       <c r="B22" s="1" t="s">
         <v>111</v>
       </c>
@@ -2486,11 +2590,15 @@
       <c r="H22" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="8"/>
+      <c r="I22" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J22" s="28">
+        <v>42891</v>
+      </c>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" ht="34">
       <c r="B23" s="1" t="s">
         <v>111</v>
       </c>
@@ -2512,11 +2620,15 @@
       <c r="H23" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="8"/>
+      <c r="I23" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J23" s="28">
+        <v>42891</v>
+      </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="2:11" ht="135.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" ht="135.75" customHeight="1">
       <c r="B24" s="24" t="s">
         <v>135</v>
       </c>
@@ -2548,7 +2660,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11">
       <c r="B25" s="1" t="s">
         <v>215</v>
       </c>
@@ -2578,7 +2690,7 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11">
       <c r="B26" s="1" t="s">
         <v>216</v>
       </c>
@@ -2608,7 +2720,7 @@
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11">
       <c r="B27" s="1" t="s">
         <v>216</v>
       </c>
@@ -2638,7 +2750,7 @@
       </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="2:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" ht="33.75" customHeight="1">
       <c r="B28" s="24" t="s">
         <v>218</v>
       </c>
@@ -2668,7 +2780,7 @@
       </c>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" ht="34">
       <c r="B29" s="24" t="s">
         <v>217</v>
       </c>
@@ -2698,7 +2810,7 @@
       </c>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" ht="51">
       <c r="B30" s="24" t="s">
         <v>219</v>
       </c>
@@ -2728,7 +2840,7 @@
       </c>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" ht="51">
       <c r="B31" s="24" t="s">
         <v>220</v>
       </c>
@@ -2758,7 +2870,7 @@
       </c>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" ht="51">
       <c r="B32" s="24" t="s">
         <v>221</v>
       </c>
@@ -2788,7 +2900,7 @@
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" ht="51">
       <c r="B33" s="24" t="s">
         <v>222</v>
       </c>
@@ -2818,7 +2930,7 @@
       </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" ht="51">
       <c r="B34" s="24" t="s">
         <v>223</v>
       </c>
@@ -2848,7 +2960,7 @@
       </c>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" ht="51">
       <c r="B35" s="24" t="s">
         <v>224</v>
       </c>
@@ -2878,7 +2990,7 @@
       </c>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" ht="51">
       <c r="B36" s="24" t="s">
         <v>226</v>
       </c>
@@ -2908,7 +3020,7 @@
       </c>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" ht="34">
       <c r="B37" s="24" t="s">
         <v>225</v>
       </c>
@@ -2938,7 +3050,7 @@
       </c>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" ht="34">
       <c r="B38" s="24" t="s">
         <v>227</v>
       </c>
@@ -2968,7 +3080,7 @@
       </c>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" ht="34">
       <c r="B39" s="24" t="s">
         <v>228</v>
       </c>
@@ -2998,7 +3110,7 @@
       </c>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>

</xml_diff>